<commit_message>
Swapped out link to cheaper (worse tolerance) part in motherboard BOM
</commit_message>
<xml_diff>
--- a/Hardware/Boards/Motherboard/Motherboard_BOM.xlsx
+++ b/Hardware/Boards/Motherboard/Motherboard_BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="14355" windowHeight="5205"/>
@@ -925,9 +925,6 @@
     <t>96M1466</t>
   </si>
   <si>
-    <t>http://www.newark.com/avx/12061c104jat2a/capacitor-ceramic-0-1uf-100v-x7r/dp/96M1466</t>
-  </si>
-  <si>
     <t>30H0930</t>
   </si>
   <si>
@@ -1220,6 +1217,9 @@
   </si>
   <si>
     <t xml:space="preserve">TOL-11300 </t>
+  </si>
+  <si>
+    <t>http://www.newark.com/yageo/cc1206krx7r9bb104/capacitor-ceramic-0-1uf-50v-x7r/dp/68R4967</t>
   </si>
 </sst>
 </file>
@@ -1750,6 +1750,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1759,13 +1766,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2112,7 +2112,7 @@
   <dimension ref="A1:I221"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I83" sqref="I83"/>
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2154,12 +2154,12 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F2" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="F2" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -2210,7 +2210,7 @@
         <v>56</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>302</v>
+        <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2227,16 +2227,16 @@
         <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H5" s="1">
         <v>1</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2253,16 +2253,16 @@
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H6" s="1">
         <v>3</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2282,13 +2282,13 @@
         <v>38</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H7" s="1">
         <v>2</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2305,16 +2305,16 @@
         <v>16</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>310</v>
       </c>
       <c r="H8" s="1">
         <v>2</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2322,7 +2322,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C9" s="2">
         <v>1206</v>
@@ -2334,13 +2334,13 @@
         <v>29</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H9" s="1">
         <v>2</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2348,7 +2348,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C10" s="2">
         <v>1206</v>
@@ -2360,13 +2360,13 @@
         <v>53</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H10" s="1">
         <v>1</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2386,13 +2386,13 @@
         <v>70</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H11" s="1">
         <v>1</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2409,16 +2409,16 @@
         <v>1206</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="G12" t="s">
         <v>345</v>
-      </c>
-      <c r="G12" t="s">
-        <v>346</v>
       </c>
       <c r="H12" s="1">
         <v>2</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2434,10 +2434,10 @@
       <c r="D13" s="2">
         <v>1206</v>
       </c>
-      <c r="F13" s="11" t="s">
-        <v>390</v>
-      </c>
-      <c r="G13" s="12"/>
+      <c r="F13" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="G13" s="9"/>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2470,12 +2470,12 @@
       <c r="D15" s="2">
         <v>1206</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="F15" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -2494,13 +2494,13 @@
         <v>120</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H16" s="1">
         <v>40</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2520,13 +2520,13 @@
         <v>154</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H17" s="1">
         <v>15</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -2546,13 +2546,13 @@
         <v>330</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H18" s="1">
         <v>3</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2572,13 +2572,13 @@
         <v>158</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H19" s="1">
         <v>4</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2598,13 +2598,13 @@
         <v>51</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H20" s="1">
         <v>4</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2624,13 +2624,13 @@
         <v>200</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H21" s="1">
         <v>2</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2650,13 +2650,13 @@
         <v>162</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H22" s="1">
         <v>1</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2673,16 +2673,16 @@
         <v>1206</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H23" s="1">
         <v>1</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2698,8 +2698,8 @@
       <c r="D24" s="2">
         <v>1206</v>
       </c>
-      <c r="F24" s="11" t="s">
-        <v>391</v>
+      <c r="F24" s="8" t="s">
+        <v>390</v>
       </c>
       <c r="G24" s="5"/>
     </row>
@@ -2731,12 +2731,12 @@
       <c r="D26" s="2">
         <v>1206</v>
       </c>
-      <c r="F26" s="8" t="s">
-        <v>338</v>
-      </c>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
+      <c r="F26" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
@@ -2752,16 +2752,16 @@
         <v>1206</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H27" s="1">
         <v>20</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2778,16 +2778,16 @@
         <v>1206</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H28" s="1">
         <v>8</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2804,16 +2804,16 @@
         <v>1206</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H29" s="1">
         <v>1</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2830,16 +2830,16 @@
         <v>1206</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H30" s="1">
         <v>1</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2859,13 +2859,13 @@
         <v>113</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H31" s="4">
         <v>1</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2885,13 +2885,13 @@
         <v>117</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H32" s="1">
         <v>1</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2908,16 +2908,16 @@
         <v>1206</v>
       </c>
       <c r="F33" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="G33" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="G33" s="4" t="s">
-        <v>364</v>
-      </c>
-      <c r="H33" s="10">
+      <c r="H33" s="7">
         <v>3</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2934,16 +2934,16 @@
         <v>1206</v>
       </c>
       <c r="F34" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>379</v>
       </c>
       <c r="H34" s="1">
         <v>1</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2960,16 +2960,16 @@
         <v>1206</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H35" s="1">
         <v>1</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -3028,12 +3028,12 @@
       <c r="D39" s="2">
         <v>1206</v>
       </c>
-      <c r="F39" s="9" t="s">
-        <v>358</v>
-      </c>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
+      <c r="F39" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -3049,16 +3049,16 @@
         <v>1206</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H40" s="1">
         <v>1</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -3075,16 +3075,16 @@
         <v>1206</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H41" s="1">
         <v>8</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -3101,16 +3101,16 @@
         <v>1206</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H42" s="1">
         <v>1</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -3127,16 +3127,16 @@
         <v>1206</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H43" s="1">
         <v>3</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -3153,16 +3153,16 @@
         <v>1206</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H44" s="1">
         <v>1</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -3179,16 +3179,16 @@
         <v>1206</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H45" s="1">
         <v>1</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -3205,16 +3205,16 @@
         <v>1206</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G46" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H46" s="1">
         <v>1</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -3231,16 +3231,16 @@
         <v>1206</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H47" s="1">
         <v>1</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -3257,16 +3257,16 @@
         <v>1206</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H48" s="1">
         <v>6</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -3422,12 +3422,12 @@
       <c r="D59" s="2">
         <v>1206</v>
       </c>
-      <c r="F59" s="7" t="s">
-        <v>392</v>
-      </c>
-      <c r="G59" s="7"/>
-      <c r="H59" s="7"/>
-      <c r="I59" s="7"/>
+      <c r="F59" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
@@ -3443,7 +3443,7 @@
         <v>1206</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -3460,7 +3460,7 @@
         <v>1206</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -5591,7 +5591,7 @@
         <v>279</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -5720,38 +5720,38 @@
     <hyperlink ref="I7" r:id="rId2"/>
     <hyperlink ref="I5" r:id="rId3"/>
     <hyperlink ref="I8" r:id="rId4"/>
-    <hyperlink ref="I4" r:id="rId5"/>
-    <hyperlink ref="I3" r:id="rId6"/>
-    <hyperlink ref="I9" r:id="rId7"/>
-    <hyperlink ref="I10" r:id="rId8"/>
-    <hyperlink ref="I11" r:id="rId9"/>
-    <hyperlink ref="I16" r:id="rId10"/>
-    <hyperlink ref="I17" r:id="rId11"/>
-    <hyperlink ref="I18" r:id="rId12"/>
-    <hyperlink ref="I19" r:id="rId13"/>
-    <hyperlink ref="I20" r:id="rId14"/>
-    <hyperlink ref="I21" r:id="rId15"/>
-    <hyperlink ref="I22" r:id="rId16"/>
-    <hyperlink ref="I23" r:id="rId17"/>
-    <hyperlink ref="I27" r:id="rId18"/>
-    <hyperlink ref="I28" r:id="rId19"/>
-    <hyperlink ref="I12" r:id="rId20"/>
-    <hyperlink ref="I29" r:id="rId21"/>
-    <hyperlink ref="I30" r:id="rId22"/>
-    <hyperlink ref="I31" r:id="rId23" location="Description"/>
-    <hyperlink ref="I32" r:id="rId24" location=".Uqtwa4bh58E"/>
-    <hyperlink ref="I40" r:id="rId25"/>
-    <hyperlink ref="I33" r:id="rId26"/>
-    <hyperlink ref="I41" r:id="rId27"/>
-    <hyperlink ref="I42" r:id="rId28"/>
-    <hyperlink ref="I43" r:id="rId29"/>
-    <hyperlink ref="I44" r:id="rId30"/>
-    <hyperlink ref="I34" r:id="rId31"/>
-    <hyperlink ref="I45" r:id="rId32"/>
-    <hyperlink ref="I35" r:id="rId33"/>
-    <hyperlink ref="I47" r:id="rId34" location="Downloads"/>
-    <hyperlink ref="I46" r:id="rId35"/>
-    <hyperlink ref="I48" r:id="rId36"/>
+    <hyperlink ref="I3" r:id="rId5"/>
+    <hyperlink ref="I9" r:id="rId6"/>
+    <hyperlink ref="I10" r:id="rId7"/>
+    <hyperlink ref="I11" r:id="rId8"/>
+    <hyperlink ref="I16" r:id="rId9"/>
+    <hyperlink ref="I17" r:id="rId10"/>
+    <hyperlink ref="I18" r:id="rId11"/>
+    <hyperlink ref="I19" r:id="rId12"/>
+    <hyperlink ref="I20" r:id="rId13"/>
+    <hyperlink ref="I21" r:id="rId14"/>
+    <hyperlink ref="I22" r:id="rId15"/>
+    <hyperlink ref="I23" r:id="rId16"/>
+    <hyperlink ref="I27" r:id="rId17"/>
+    <hyperlink ref="I28" r:id="rId18"/>
+    <hyperlink ref="I12" r:id="rId19"/>
+    <hyperlink ref="I29" r:id="rId20"/>
+    <hyperlink ref="I30" r:id="rId21"/>
+    <hyperlink ref="I31" r:id="rId22" location="Description"/>
+    <hyperlink ref="I32" r:id="rId23" location=".Uqtwa4bh58E"/>
+    <hyperlink ref="I40" r:id="rId24"/>
+    <hyperlink ref="I33" r:id="rId25"/>
+    <hyperlink ref="I41" r:id="rId26"/>
+    <hyperlink ref="I42" r:id="rId27"/>
+    <hyperlink ref="I43" r:id="rId28"/>
+    <hyperlink ref="I44" r:id="rId29"/>
+    <hyperlink ref="I34" r:id="rId30"/>
+    <hyperlink ref="I45" r:id="rId31"/>
+    <hyperlink ref="I35" r:id="rId32"/>
+    <hyperlink ref="I47" r:id="rId33" location="Downloads"/>
+    <hyperlink ref="I46" r:id="rId34"/>
+    <hyperlink ref="I48" r:id="rId35"/>
+    <hyperlink ref="I4" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId37"/>

</xml_diff>

<commit_message>
Added a found column to the motherboard stuff.
</commit_message>
<xml_diff>
--- a/Hardware/Boards/Motherboard/Motherboard_BOM.xlsx
+++ b/Hardware/Boards/Motherboard/Motherboard_BOM.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="14355" windowHeight="5205"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="14355" windowHeight="5205" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Motherboard" sheetId="1" r:id="rId1"/>
+    <sheet name="Parts Received" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Motherboard!$A$1:$D$221</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="418">
   <si>
     <t>Part</t>
   </si>
@@ -1265,6 +1266,12 @@
   </si>
   <si>
     <t>Green SMD Leds</t>
+  </si>
+  <si>
+    <t>Received</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -1416,7 +1423,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1608,6 +1615,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1779,7 +1792,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1795,6 +1808,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1804,13 +1824,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2156,8 +2172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I221"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F57" sqref="F1:I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2199,12 +2215,12 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2479,7 +2495,7 @@
       <c r="D13" s="2">
         <v>1206</v>
       </c>
-      <c r="F13" s="10"/>
+      <c r="F13" s="7"/>
       <c r="G13" s="5"/>
       <c r="I13" s="3"/>
     </row>
@@ -2513,12 +2529,12 @@
       <c r="D15" s="2">
         <v>1206</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -2772,12 +2788,12 @@
       <c r="D26" s="2">
         <v>1206</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
@@ -3081,12 +3097,12 @@
       <c r="D39" s="2">
         <v>1206</v>
       </c>
-      <c r="F39" s="9" t="s">
+      <c r="F39" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -3433,12 +3449,12 @@
       <c r="D53" s="2">
         <v>1206</v>
       </c>
-      <c r="F53" s="11" t="s">
+      <c r="F53" s="8" t="s">
         <v>408</v>
       </c>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
-      <c r="I53" s="12"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="9"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
@@ -3535,12 +3551,12 @@
       <c r="D59" s="2">
         <v>1206</v>
       </c>
-      <c r="F59" s="7" t="s">
+      <c r="F59" s="10" t="s">
         <v>388</v>
       </c>
-      <c r="G59" s="7"/>
-      <c r="H59" s="7"/>
-      <c r="I59" s="7"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
@@ -5882,4 +5898,864 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId42"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="99.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D3" s="1">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D4" s="1">
+        <v>57</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C12" t="s">
+        <v>345</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>120</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D16" s="1">
+        <v>40</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D17" s="1">
+        <v>15</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>330</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D19" s="1">
+        <v>8</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>51</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D20" s="1">
+        <v>4</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>200</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D27" s="1">
+        <v>20</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D28" s="1">
+        <v>8</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="D33" s="6">
+        <v>3</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C38" s="1"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="D41" s="1">
+        <v>8</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="D43" s="1">
+        <v>3</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" t="s">
+        <v>382</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="D48" s="1">
+        <v>6</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="1">
+        <v>4</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1">
+        <v>4</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1">
+        <v>1</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="9"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A39:E39"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E6" r:id="rId1"/>
+    <hyperlink ref="E7" r:id="rId2"/>
+    <hyperlink ref="E5" r:id="rId3"/>
+    <hyperlink ref="E8" r:id="rId4"/>
+    <hyperlink ref="E3" r:id="rId5"/>
+    <hyperlink ref="E9" r:id="rId6"/>
+    <hyperlink ref="E10" r:id="rId7"/>
+    <hyperlink ref="E11" r:id="rId8"/>
+    <hyperlink ref="E16" r:id="rId9"/>
+    <hyperlink ref="E17" r:id="rId10"/>
+    <hyperlink ref="E18" r:id="rId11"/>
+    <hyperlink ref="E19" r:id="rId12"/>
+    <hyperlink ref="E20" r:id="rId13"/>
+    <hyperlink ref="E21" r:id="rId14"/>
+    <hyperlink ref="E22" r:id="rId15"/>
+    <hyperlink ref="E23" r:id="rId16"/>
+    <hyperlink ref="E27" r:id="rId17"/>
+    <hyperlink ref="E28" r:id="rId18"/>
+    <hyperlink ref="E12" r:id="rId19"/>
+    <hyperlink ref="E29" r:id="rId20"/>
+    <hyperlink ref="E30" r:id="rId21"/>
+    <hyperlink ref="E31" r:id="rId22" location="Description"/>
+    <hyperlink ref="E32" r:id="rId23" location=".Uqtwa4bh58E"/>
+    <hyperlink ref="E40" r:id="rId24"/>
+    <hyperlink ref="E33" r:id="rId25"/>
+    <hyperlink ref="E41" r:id="rId26"/>
+    <hyperlink ref="E42" r:id="rId27"/>
+    <hyperlink ref="E43" r:id="rId28"/>
+    <hyperlink ref="E44" r:id="rId29"/>
+    <hyperlink ref="E34" r:id="rId30"/>
+    <hyperlink ref="E45" r:id="rId31"/>
+    <hyperlink ref="E35" r:id="rId32"/>
+    <hyperlink ref="E47" r:id="rId33" location="Downloads"/>
+    <hyperlink ref="E46" r:id="rId34"/>
+    <hyperlink ref="E48" r:id="rId35"/>
+    <hyperlink ref="E4" r:id="rId36"/>
+    <hyperlink ref="E36" r:id="rId37"/>
+    <hyperlink ref="E49" r:id="rId38"/>
+    <hyperlink ref="E50" r:id="rId39"/>
+    <hyperlink ref="E51" r:id="rId40"/>
+    <hyperlink ref="E52" r:id="rId41"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated what we have section.
</commit_message>
<xml_diff>
--- a/Hardware/Boards/Motherboard/Motherboard_BOM.xlsx
+++ b/Hardware/Boards/Motherboard/Motherboard_BOM.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="421">
   <si>
     <t>Part</t>
   </si>
@@ -1272,6 +1272,15 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Programmer Arm</t>
+  </si>
+  <si>
+    <t>AVR Programmer</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -1423,7 +1432,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1621,6 +1630,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1792,7 +1807,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1815,6 +1830,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1824,7 +1842,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2215,12 +2234,12 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2529,12 +2548,12 @@
       <c r="D15" s="2">
         <v>1206</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -2788,12 +2807,12 @@
       <c r="D26" s="2">
         <v>1206</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="12" t="s">
         <v>337</v>
       </c>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
@@ -3097,12 +3116,12 @@
       <c r="D39" s="2">
         <v>1206</v>
       </c>
-      <c r="F39" s="12" t="s">
+      <c r="F39" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -3551,12 +3570,12 @@
       <c r="D59" s="2">
         <v>1206</v>
       </c>
-      <c r="F59" s="10" t="s">
+      <c r="F59" s="11" t="s">
         <v>388</v>
       </c>
-      <c r="G59" s="10"/>
-      <c r="H59" s="10"/>
-      <c r="I59" s="10"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="11"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
@@ -5902,10 +5921,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5934,19 +5953,19 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="10" t="s">
         <v>417</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -5963,8 +5982,8 @@
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>417</v>
+      <c r="B4" s="15" t="s">
+        <v>420</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>301</v>
@@ -5980,7 +5999,7 @@
       <c r="A5" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="10" t="s">
         <v>417</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -5997,7 +6016,7 @@
       <c r="A6" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="10" t="s">
         <v>417</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -6014,7 +6033,7 @@
       <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="10" t="s">
         <v>417</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -6031,8 +6050,8 @@
       <c r="A8" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>417</v>
+      <c r="B8" s="15" t="s">
+        <v>420</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>309</v>
@@ -6048,8 +6067,8 @@
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>417</v>
+      <c r="B9" s="15" t="s">
+        <v>420</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>312</v>
@@ -6065,8 +6084,8 @@
       <c r="A10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>417</v>
+      <c r="B10" s="15" t="s">
+        <v>420</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>314</v>
@@ -6082,8 +6101,8 @@
       <c r="A11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>417</v>
+      <c r="B11" s="15" t="s">
+        <v>420</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>317</v>
@@ -6099,8 +6118,8 @@
       <c r="A12" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>417</v>
+      <c r="B12" s="15" t="s">
+        <v>420</v>
       </c>
       <c r="C12" t="s">
         <v>345</v>
@@ -6126,20 +6145,20 @@
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>120</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>417</v>
+      <c r="B16" s="15" t="s">
+        <v>420</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>320</v>
@@ -6155,7 +6174,7 @@
       <c r="A17" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="10" t="s">
         <v>417</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -6172,7 +6191,7 @@
       <c r="A18" s="4">
         <v>330</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="10" t="s">
         <v>417</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -6189,7 +6208,7 @@
       <c r="A19" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="10" t="s">
         <v>417</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -6206,7 +6225,7 @@
       <c r="A20" s="4">
         <v>51</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="10" t="s">
         <v>417</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -6223,7 +6242,7 @@
       <c r="A21" s="4">
         <v>200</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="10" t="s">
         <v>417</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -6240,7 +6259,7 @@
       <c r="A22" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="10" t="s">
         <v>417</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -6257,7 +6276,7 @@
       <c r="A23" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="10" t="s">
         <v>417</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -6283,19 +6302,21 @@
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="12" t="s">
         <v>337</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="B27" s="4"/>
+      <c r="B27" s="10" t="s">
+        <v>417</v>
+      </c>
       <c r="C27" s="1" t="s">
         <v>338</v>
       </c>
@@ -6310,7 +6331,9 @@
       <c r="A28" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="B28" s="4"/>
+      <c r="B28" s="10" t="s">
+        <v>417</v>
+      </c>
       <c r="C28" s="1" t="s">
         <v>341</v>
       </c>
@@ -6325,7 +6348,9 @@
       <c r="A29" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="B29" s="4"/>
+      <c r="B29" s="10" t="s">
+        <v>417</v>
+      </c>
       <c r="C29" s="1" t="s">
         <v>347</v>
       </c>
@@ -6340,7 +6365,9 @@
       <c r="A30" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="B30" s="4"/>
+      <c r="B30" s="10" t="s">
+        <v>417</v>
+      </c>
       <c r="C30" s="1" t="s">
         <v>350</v>
       </c>
@@ -6355,7 +6382,9 @@
       <c r="A31" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B31" s="4"/>
+      <c r="B31" s="15" t="s">
+        <v>420</v>
+      </c>
       <c r="C31" s="4" t="s">
         <v>353</v>
       </c>
@@ -6370,7 +6399,9 @@
       <c r="A32" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B32" s="4"/>
+      <c r="B32" s="15" t="s">
+        <v>420</v>
+      </c>
       <c r="C32" s="4" t="s">
         <v>356</v>
       </c>
@@ -6385,7 +6416,9 @@
       <c r="A33" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="B33" s="4"/>
+      <c r="B33" s="10" t="s">
+        <v>417</v>
+      </c>
       <c r="C33" s="4" t="s">
         <v>363</v>
       </c>
@@ -6400,7 +6433,9 @@
       <c r="A34" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="B34" s="4"/>
+      <c r="B34" s="10" t="s">
+        <v>417</v>
+      </c>
       <c r="C34" s="1" t="s">
         <v>378</v>
       </c>
@@ -6415,7 +6450,7 @@
       <c r="A35" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="10" t="s">
         <v>417</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -6432,7 +6467,7 @@
       <c r="A36" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="10" t="s">
         <v>417</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -6454,19 +6489,19 @@
       <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="10" t="s">
         <v>417</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -6483,7 +6518,9 @@
       <c r="A41" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="B41" s="1"/>
+      <c r="B41" s="10" t="s">
+        <v>417</v>
+      </c>
       <c r="C41" s="1" t="s">
         <v>364</v>
       </c>
@@ -6498,7 +6535,9 @@
       <c r="A42" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="B42" s="1"/>
+      <c r="B42" s="10" t="s">
+        <v>417</v>
+      </c>
       <c r="C42" s="1" t="s">
         <v>367</v>
       </c>
@@ -6513,7 +6552,9 @@
       <c r="A43" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="B43" s="1"/>
+      <c r="B43" s="15" t="s">
+        <v>420</v>
+      </c>
       <c r="C43" s="1" t="s">
         <v>370</v>
       </c>
@@ -6528,7 +6569,9 @@
       <c r="A44" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="B44" s="1"/>
+      <c r="B44" s="15" t="s">
+        <v>420</v>
+      </c>
       <c r="C44" s="1" t="s">
         <v>373</v>
       </c>
@@ -6543,7 +6586,7 @@
       <c r="A45" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="10" t="s">
         <v>417</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -6560,7 +6603,9 @@
       <c r="A46" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="B46" s="1"/>
+      <c r="B46" s="15" t="s">
+        <v>420</v>
+      </c>
       <c r="C46" t="s">
         <v>382</v>
       </c>
@@ -6575,7 +6620,9 @@
       <c r="A47" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="B47" s="1"/>
+      <c r="B47" s="15" t="s">
+        <v>420</v>
+      </c>
       <c r="C47" s="1" t="s">
         <v>392</v>
       </c>
@@ -6590,7 +6637,7 @@
       <c r="A48" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="B48" s="10" t="s">
         <v>417</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -6607,7 +6654,9 @@
       <c r="A49" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="B49" s="1"/>
+      <c r="B49" s="15" t="s">
+        <v>420</v>
+      </c>
       <c r="C49" s="1" t="s">
         <v>6</v>
       </c>
@@ -6622,7 +6671,7 @@
       <c r="A50" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="10" t="s">
         <v>417</v>
       </c>
       <c r="C50" s="1"/>
@@ -6637,7 +6686,7 @@
       <c r="A51" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="B51" s="13" t="s">
+      <c r="B51" s="10" t="s">
         <v>417</v>
       </c>
       <c r="C51" s="1"/>
@@ -6652,7 +6701,7 @@
       <c r="A52" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="B52" s="13" t="s">
+      <c r="B52" s="10" t="s">
         <v>417</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -6678,7 +6727,9 @@
       <c r="A54" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="B54" s="1"/>
+      <c r="B54" s="10" t="s">
+        <v>417</v>
+      </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
     </row>
@@ -6705,6 +6756,22 @@
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>420</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Forgot what I changed.
</commit_message>
<xml_diff>
--- a/Hardware/Boards/Motherboard/Motherboard_BOM.xlsx
+++ b/Hardware/Boards/Motherboard/Motherboard_BOM.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="419">
   <si>
     <t>Part</t>
   </si>
@@ -1272,12 +1272,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>Programmer Arm</t>
-  </si>
-  <si>
-    <t>AVR Programmer</t>
   </si>
   <si>
     <t>No</t>
@@ -1807,7 +1801,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1833,6 +1827,9 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1840,10 +1837,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2234,12 +2227,12 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="12" t="s">
         <v>318</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2548,12 +2541,12 @@
       <c r="D15" s="2">
         <v>1206</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="12" t="s">
         <v>319</v>
       </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -2807,12 +2800,12 @@
       <c r="D26" s="2">
         <v>1206</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
@@ -3116,12 +3109,12 @@
       <c r="D39" s="2">
         <v>1206</v>
       </c>
-      <c r="F39" s="13" t="s">
+      <c r="F39" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -3570,12 +3563,12 @@
       <c r="D59" s="2">
         <v>1206</v>
       </c>
-      <c r="F59" s="11" t="s">
+      <c r="F59" s="12" t="s">
         <v>388</v>
       </c>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11"/>
-      <c r="I59" s="11"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="12"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
@@ -5921,10 +5914,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5953,13 +5946,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -5982,8 +5975,8 @@
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>420</v>
+      <c r="B4" s="11" t="s">
+        <v>418</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>301</v>
@@ -6050,8 +6043,8 @@
       <c r="A8" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>420</v>
+      <c r="B8" s="11" t="s">
+        <v>418</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>309</v>
@@ -6067,8 +6060,8 @@
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>420</v>
+      <c r="B9" s="11" t="s">
+        <v>418</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>312</v>
@@ -6084,8 +6077,8 @@
       <c r="A10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>420</v>
+      <c r="B10" s="11" t="s">
+        <v>418</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>314</v>
@@ -6101,8 +6094,8 @@
       <c r="A11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>420</v>
+      <c r="B11" s="11" t="s">
+        <v>418</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>317</v>
@@ -6118,8 +6111,8 @@
       <c r="A12" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>420</v>
+      <c r="B12" s="11" t="s">
+        <v>418</v>
       </c>
       <c r="C12" t="s">
         <v>345</v>
@@ -6145,20 +6138,20 @@
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="12" t="s">
         <v>319</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>120</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>420</v>
+      <c r="B16" s="11" t="s">
+        <v>418</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>320</v>
@@ -6302,13 +6295,13 @@
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
@@ -6382,8 +6375,8 @@
       <c r="A31" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B31" s="15" t="s">
-        <v>420</v>
+      <c r="B31" s="11" t="s">
+        <v>418</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>353</v>
@@ -6399,8 +6392,8 @@
       <c r="A32" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B32" s="15" t="s">
-        <v>420</v>
+      <c r="B32" s="11" t="s">
+        <v>418</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>356</v>
@@ -6489,13 +6482,13 @@
       <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
@@ -6552,8 +6545,8 @@
       <c r="A43" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="B43" s="15" t="s">
-        <v>420</v>
+      <c r="B43" s="11" t="s">
+        <v>418</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>370</v>
@@ -6569,8 +6562,8 @@
       <c r="A44" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="B44" s="15" t="s">
-        <v>420</v>
+      <c r="B44" s="11" t="s">
+        <v>418</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>373</v>
@@ -6586,8 +6579,8 @@
       <c r="A45" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="B45" s="10" t="s">
-        <v>417</v>
+      <c r="B45" s="11" t="s">
+        <v>418</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>379</v>
@@ -6603,8 +6596,8 @@
       <c r="A46" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="B46" s="15" t="s">
-        <v>420</v>
+      <c r="B46" s="11" t="s">
+        <v>418</v>
       </c>
       <c r="C46" t="s">
         <v>382</v>
@@ -6620,8 +6613,8 @@
       <c r="A47" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="B47" s="15" t="s">
-        <v>420</v>
+      <c r="B47" s="11" t="s">
+        <v>418</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>392</v>
@@ -6654,8 +6647,8 @@
       <c r="A49" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="B49" s="15" t="s">
-        <v>420</v>
+      <c r="B49" s="11" t="s">
+        <v>418</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>6</v>
@@ -6715,27 +6708,26 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
-        <v>408</v>
-      </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="9"/>
+      <c r="A53" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="B54" s="10" t="s">
-        <v>417</v>
-      </c>
+        <v>413</v>
+      </c>
+      <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -6743,35 +6735,11 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="B59" s="14" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>420</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>